<commit_message>
Added energy balance calculations, option visuals
-Added energyAsset with connectivity and energy balance
-Added Building connectivity and energy balance
-Added node energy balance
-Added KPI-visuals for nodes
</commit_message>
<xml_diff>
--- a/Base/db_backboneConfig.xlsx
+++ b/Base/db_backboneConfig.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\HOUJ\Documents\GitHub\HOLON\Base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5DBB900-630D-40DD-83C4-D0E911B53608}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF46B540-2DB7-492C-940B-293AF9DA59F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" xr2:uid="{C61B0771-0652-4F35-8DF1-D2D550B8F66D}"/>
+    <workbookView xWindow="1530" yWindow="18210" windowWidth="13065" windowHeight="11385" xr2:uid="{C61B0771-0652-4F35-8DF1-D2D550B8F66D}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="41">
   <si>
     <t>id</t>
   </si>
@@ -149,6 +149,15 @@
   </si>
   <si>
     <t>production</t>
+  </si>
+  <si>
+    <t>windmolen</t>
+  </si>
+  <si>
+    <t>b10</t>
+  </si>
+  <si>
+    <t>b11</t>
   </si>
 </sst>
 </file>
@@ -500,16 +509,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1488AC62-2553-41A1-BF66-2CB68340C396}">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="12.1640625" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -856,22 +866,20 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="C16" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="D16" t="s">
-        <v>37</v>
-      </c>
-      <c r="E16" t="s">
         <v>36</v>
       </c>
       <c r="F16" t="s">
-        <v>3</v>
-      </c>
-      <c r="G16">
-        <v>30000</v>
+        <v>2</v>
+      </c>
+      <c r="G16" s="1">
+        <f>400*1000</f>
+        <v>400000</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -879,22 +887,20 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="C17" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="D17" t="s">
-        <v>37</v>
-      </c>
-      <c r="E17" t="s">
         <v>36</v>
       </c>
       <c r="F17" t="s">
         <v>3</v>
       </c>
-      <c r="G17">
-        <v>6000</v>
+      <c r="G17" s="1">
+        <f>400*1000</f>
+        <v>400000</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -905,18 +911,64 @@
         <v>32</v>
       </c>
       <c r="C18" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D18" t="s">
         <v>37</v>
       </c>
       <c r="E18" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F18" t="s">
-        <v>4</v>
+        <v>39</v>
       </c>
       <c r="G18">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" t="s">
+        <v>37</v>
+      </c>
+      <c r="E19" t="s">
+        <v>38</v>
+      </c>
+      <c r="F19" t="s">
+        <v>39</v>
+      </c>
+      <c r="G19">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" t="s">
+        <v>37</v>
+      </c>
+      <c r="E20" t="s">
+        <v>38</v>
+      </c>
+      <c r="F20" t="s">
+        <v>40</v>
+      </c>
+      <c r="G20">
         <v>40000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixes energiebalansen toevoegingen visuals
-Energiebalansen NetNodes worden nu ook uitgerekend voor onderliggende nodes
-Optionele KPI-agent tekent flexibel NetNode-stations op het juiste level
-Agentlinks in KPI-agent ter illustratie van systeemconfiguratie
-Weergave van realtime netto elektriciteitsstromen per netstation in KPI-agent ter checking en debugging
</commit_message>
<xml_diff>
--- a/Base/db_backboneConfig.xlsx
+++ b/Base/db_backboneConfig.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\HOUJ\Documents\GitHub\HOLON\Base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF46B540-2DB7-492C-940B-293AF9DA59F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C135CA2F-B478-4FEC-BF78-0AC333137777}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1530" yWindow="18210" windowWidth="13065" windowHeight="11385" xr2:uid="{C61B0771-0652-4F35-8DF1-D2D550B8F66D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C61B0771-0652-4F35-8DF1-D2D550B8F66D}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" r:id="rId1"/>
@@ -512,13 +512,14 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="12.1640625" customWidth="1"/>
+    <col min="2" max="2" width="19" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" customWidth="1"/>
     <col min="7" max="7" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -875,7 +876,7 @@
         <v>36</v>
       </c>
       <c r="F16" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G16" s="1">
         <f>400*1000</f>
@@ -896,7 +897,7 @@
         <v>36</v>
       </c>
       <c r="F17" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G17" s="1">
         <f>400*1000</f>

</xml_diff>

<commit_message>
Extended building categories and visualisations
Houses, stores, offices and windfarms, solarfarms zijn nu zichtbaar met bijbehorende icoontjes en placement in de KPI-agent zodat backbone-configuratie makkelijk gecheckt kan worden.

-excel-file configuratie aangepast met meer huizen, gebouwen (winkel, kantoor) en solarfarm 'Building' en solarpanel EnergyAsset
</commit_message>
<xml_diff>
--- a/Base/db_backboneConfig.xlsx
+++ b/Base/db_backboneConfig.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\HOUJ\Documents\GitHub\HOLON\Base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C135CA2F-B478-4FEC-BF78-0AC333137777}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75C2DCC8-F399-4EB2-8738-DD9069D04E04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C61B0771-0652-4F35-8DF1-D2D550B8F66D}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{C61B0771-0652-4F35-8DF1-D2D550B8F66D}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="62">
   <si>
     <t>id</t>
   </si>
@@ -145,29 +145,97 @@
     <t>a3</t>
   </si>
   <si>
-    <t>windpark</t>
-  </si>
-  <si>
     <t>production</t>
   </si>
   <si>
-    <t>windmolen</t>
-  </si>
-  <si>
     <t>b10</t>
   </si>
   <si>
     <t>b11</t>
+  </si>
+  <si>
+    <t>windfarm</t>
+  </si>
+  <si>
+    <t>b12</t>
+  </si>
+  <si>
+    <t>solarfarm</t>
+  </si>
+  <si>
+    <t>store</t>
+  </si>
+  <si>
+    <t>b13</t>
+  </si>
+  <si>
+    <t>b14</t>
+  </si>
+  <si>
+    <t>b15</t>
+  </si>
+  <si>
+    <t>b16</t>
+  </si>
+  <si>
+    <t>b17</t>
+  </si>
+  <si>
+    <t>b18</t>
+  </si>
+  <si>
+    <t>b19</t>
+  </si>
+  <si>
+    <t>b20</t>
+  </si>
+  <si>
+    <t>b21</t>
+  </si>
+  <si>
+    <t>b22</t>
+  </si>
+  <si>
+    <t>b23</t>
+  </si>
+  <si>
+    <t>b24</t>
+  </si>
+  <si>
+    <t>b25</t>
+  </si>
+  <si>
+    <t>a4</t>
+  </si>
+  <si>
+    <t>windmill</t>
+  </si>
+  <si>
+    <t>solarpanel</t>
+  </si>
+  <si>
+    <t>office</t>
+  </si>
+  <si>
+    <t>b26</t>
+  </si>
+  <si>
+    <t>b27</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="9"/>
       <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
@@ -509,10 +577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1488AC62-2553-41A1-BF66-2CB68340C396}">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -870,17 +938,19 @@
         <v>18</v>
       </c>
       <c r="C16" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D16" t="s">
-        <v>36</v>
+        <v>28</v>
+      </c>
+      <c r="E16" t="s">
+        <v>29</v>
       </c>
       <c r="F16" t="s">
         <v>3</v>
       </c>
       <c r="G16" s="1">
-        <f>400*1000</f>
-        <v>400000</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -891,17 +961,19 @@
         <v>18</v>
       </c>
       <c r="C17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D17" t="s">
-        <v>36</v>
+        <v>28</v>
+      </c>
+      <c r="E17" t="s">
+        <v>30</v>
       </c>
       <c r="F17" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G17" s="1">
-        <f>400*1000</f>
-        <v>400000</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -909,22 +981,22 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="C18" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="D18" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="E18" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="F18" t="s">
-        <v>39</v>
-      </c>
-      <c r="G18">
-        <v>30000</v>
+        <v>3</v>
+      </c>
+      <c r="G18" s="1">
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -932,22 +1004,22 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="D19" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="E19" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="F19" t="s">
-        <v>39</v>
-      </c>
-      <c r="G19">
-        <v>6000</v>
+        <v>4</v>
+      </c>
+      <c r="G19" s="1">
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -955,25 +1027,410 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" t="s">
+        <v>28</v>
+      </c>
+      <c r="E20" t="s">
+        <v>31</v>
+      </c>
+      <c r="F20" t="s">
+        <v>4</v>
+      </c>
+      <c r="G20" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" t="s">
+        <v>28</v>
+      </c>
+      <c r="E21" t="s">
+        <v>30</v>
+      </c>
+      <c r="F21" t="s">
+        <v>4</v>
+      </c>
+      <c r="G21" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" t="s">
+        <v>28</v>
+      </c>
+      <c r="E22" t="s">
+        <v>30</v>
+      </c>
+      <c r="F22" t="s">
+        <v>6</v>
+      </c>
+      <c r="G22" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" t="s">
+        <v>47</v>
+      </c>
+      <c r="D23" t="s">
+        <v>28</v>
+      </c>
+      <c r="E23" t="s">
+        <v>29</v>
+      </c>
+      <c r="F23" t="s">
+        <v>6</v>
+      </c>
+      <c r="G23" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" t="s">
+        <v>48</v>
+      </c>
+      <c r="D24" t="s">
+        <v>28</v>
+      </c>
+      <c r="E24" t="s">
+        <v>29</v>
+      </c>
+      <c r="F24" t="s">
+        <v>6</v>
+      </c>
+      <c r="G24" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25" t="s">
+        <v>49</v>
+      </c>
+      <c r="D25" t="s">
+        <v>18</v>
+      </c>
+      <c r="E25" t="s">
+        <v>42</v>
+      </c>
+      <c r="F25" t="s">
+        <v>3</v>
+      </c>
+      <c r="G25" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" t="s">
+        <v>50</v>
+      </c>
+      <c r="D26" t="s">
+        <v>18</v>
+      </c>
+      <c r="E26" t="s">
+        <v>42</v>
+      </c>
+      <c r="F26" t="s">
+        <v>4</v>
+      </c>
+      <c r="G26" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27" t="s">
+        <v>51</v>
+      </c>
+      <c r="D27" t="s">
+        <v>18</v>
+      </c>
+      <c r="E27" t="s">
+        <v>42</v>
+      </c>
+      <c r="F27" t="s">
+        <v>6</v>
+      </c>
+      <c r="G27" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28" t="s">
+        <v>52</v>
+      </c>
+      <c r="D28" t="s">
+        <v>18</v>
+      </c>
+      <c r="E28" t="s">
+        <v>42</v>
+      </c>
+      <c r="F28" t="s">
+        <v>3</v>
+      </c>
+      <c r="G28" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>18</v>
+      </c>
+      <c r="C29" t="s">
+        <v>53</v>
+      </c>
+      <c r="D29" t="s">
+        <v>18</v>
+      </c>
+      <c r="E29" t="s">
+        <v>59</v>
+      </c>
+      <c r="F29" t="s">
+        <v>4</v>
+      </c>
+      <c r="G29" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>18</v>
+      </c>
+      <c r="C30" t="s">
+        <v>54</v>
+      </c>
+      <c r="D30" t="s">
+        <v>18</v>
+      </c>
+      <c r="E30" t="s">
+        <v>59</v>
+      </c>
+      <c r="F30" t="s">
+        <v>6</v>
+      </c>
+      <c r="G30" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>27</v>
+      </c>
+      <c r="B31" t="s">
+        <v>18</v>
+      </c>
+      <c r="C31" t="s">
+        <v>55</v>
+      </c>
+      <c r="D31" t="s">
+        <v>39</v>
+      </c>
+      <c r="F31" t="s">
+        <v>3</v>
+      </c>
+      <c r="G31" s="1">
+        <f>400*1000</f>
+        <v>400000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>28</v>
+      </c>
+      <c r="B32" t="s">
+        <v>18</v>
+      </c>
+      <c r="C32" t="s">
+        <v>60</v>
+      </c>
+      <c r="D32" t="s">
+        <v>39</v>
+      </c>
+      <c r="F32" t="s">
+        <v>4</v>
+      </c>
+      <c r="G32" s="1">
+        <f>400*1000</f>
+        <v>400000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>29</v>
+      </c>
+      <c r="B33" t="s">
+        <v>18</v>
+      </c>
+      <c r="C33" t="s">
+        <v>61</v>
+      </c>
+      <c r="D33" t="s">
+        <v>41</v>
+      </c>
+      <c r="F33" t="s">
+        <v>6</v>
+      </c>
+      <c r="G33" s="1">
+        <f>400*1000</f>
+        <v>400000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>30</v>
+      </c>
+      <c r="B34" t="s">
         <v>32</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C34" t="s">
+        <v>33</v>
+      </c>
+      <c r="D34" t="s">
+        <v>36</v>
+      </c>
+      <c r="E34" t="s">
+        <v>57</v>
+      </c>
+      <c r="F34" t="str">
+        <f>C31</f>
+        <v>b25</v>
+      </c>
+      <c r="G34">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>31</v>
+      </c>
+      <c r="B35" t="s">
+        <v>32</v>
+      </c>
+      <c r="C35" t="s">
+        <v>34</v>
+      </c>
+      <c r="D35" t="s">
+        <v>36</v>
+      </c>
+      <c r="E35" t="s">
+        <v>57</v>
+      </c>
+      <c r="F35" t="str">
+        <f>C32</f>
+        <v>b26</v>
+      </c>
+      <c r="G35">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>32</v>
+      </c>
+      <c r="B36" t="s">
+        <v>32</v>
+      </c>
+      <c r="C36" t="s">
         <v>35</v>
       </c>
-      <c r="D20" t="s">
-        <v>37</v>
-      </c>
-      <c r="E20" t="s">
-        <v>38</v>
-      </c>
-      <c r="F20" t="s">
-        <v>40</v>
-      </c>
-      <c r="G20">
+      <c r="D36" t="s">
+        <v>36</v>
+      </c>
+      <c r="E36" t="s">
+        <v>57</v>
+      </c>
+      <c r="F36" t="str">
+        <f>C32</f>
+        <v>b26</v>
+      </c>
+      <c r="G36">
         <v>40000</v>
       </c>
     </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>33</v>
+      </c>
+      <c r="B37" t="s">
+        <v>32</v>
+      </c>
+      <c r="C37" t="s">
+        <v>56</v>
+      </c>
+      <c r="D37" t="s">
+        <v>36</v>
+      </c>
+      <c r="E37" t="s">
+        <v>58</v>
+      </c>
+      <c r="F37" t="str">
+        <f>C33</f>
+        <v>b27</v>
+      </c>
+      <c r="G37">
+        <f>300/1000*100</f>
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
BuildingAgents reformatted to NetConnection Agents
BuildingAgents are now consistently named NetConnection agents, with subtypes denoting different types such as houses, buildings or solar and windfarms.
</commit_message>
<xml_diff>
--- a/Base/db_backboneConfig.xlsx
+++ b/Base/db_backboneConfig.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\HOUJ\Documents\GitHub\HOLON\Base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75C2DCC8-F399-4EB2-8738-DD9069D04E04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE5118DB-1D80-4E83-8F59-90BD441610A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{C61B0771-0652-4F35-8DF1-D2D550B8F66D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C61B0771-0652-4F35-8DF1-D2D550B8F66D}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="63">
   <si>
     <t>id</t>
   </si>
@@ -221,6 +221,9 @@
   </si>
   <si>
     <t>b27</t>
+  </si>
+  <si>
+    <t>netConnection</t>
   </si>
 </sst>
 </file>
@@ -579,8 +582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1488AC62-2553-41A1-BF66-2CB68340C396}">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -728,7 +731,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="C7" t="s">
         <v>19</v>
@@ -751,7 +754,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="C8" t="s">
         <v>20</v>
@@ -774,7 +777,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="C9" t="s">
         <v>21</v>
@@ -797,7 +800,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="C10" t="s">
         <v>22</v>
@@ -820,7 +823,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="C11" t="s">
         <v>23</v>
@@ -843,7 +846,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="C12" t="s">
         <v>24</v>
@@ -866,7 +869,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="C13" t="s">
         <v>25</v>
@@ -889,7 +892,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="C14" t="s">
         <v>26</v>
@@ -912,7 +915,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="C15" t="s">
         <v>27</v>
@@ -935,7 +938,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="C16" t="s">
         <v>37</v>
@@ -958,7 +961,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="C17" t="s">
         <v>38</v>
@@ -981,7 +984,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="C18" t="s">
         <v>40</v>
@@ -1004,7 +1007,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="C19" t="s">
         <v>43</v>
@@ -1027,7 +1030,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="C20" t="s">
         <v>44</v>
@@ -1050,7 +1053,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="C21" t="s">
         <v>45</v>
@@ -1073,7 +1076,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="C22" t="s">
         <v>46</v>
@@ -1096,7 +1099,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="C23" t="s">
         <v>47</v>
@@ -1119,7 +1122,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="C24" t="s">
         <v>48</v>
@@ -1142,7 +1145,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="C25" t="s">
         <v>49</v>
@@ -1165,7 +1168,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="C26" t="s">
         <v>50</v>
@@ -1188,7 +1191,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="C27" t="s">
         <v>51</v>
@@ -1211,7 +1214,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="C28" t="s">
         <v>52</v>
@@ -1231,7 +1234,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="C29" t="s">
         <v>53</v>
@@ -1251,7 +1254,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="C30" t="s">
         <v>54</v>
@@ -1274,7 +1277,7 @@
         <v>27</v>
       </c>
       <c r="B31" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="C31" t="s">
         <v>55</v>
@@ -1295,7 +1298,7 @@
         <v>28</v>
       </c>
       <c r="B32" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="C32" t="s">
         <v>60</v>
@@ -1316,7 +1319,7 @@
         <v>29</v>
       </c>
       <c r="B33" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="C33" t="s">
         <v>61</v>

</xml_diff>

<commit_message>
Add basic energyAssets to NetConnections explicitly
Alternative way to add basic energyAssets to NetConnection agents without using nested agents.
-Easier to profile model startup speed in the future
-Only one energyAsset population, in main
-Flexibility: two ways of adding energyAssets, 1) from the configuration excel (for e.g. windfarms), 2) easily and explicitly define netConnection-specific energyAssets in main.
</commit_message>
<xml_diff>
--- a/Base/db_backboneConfig.xlsx
+++ b/Base/db_backboneConfig.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\HOUJ\Documents\GitHub\HOLON\Base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE5118DB-1D80-4E83-8F59-90BD441610A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E8D32AA-EE99-409D-8F25-1F7C25F05B31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C61B0771-0652-4F35-8DF1-D2D550B8F66D}"/>
   </bookViews>
@@ -582,8 +582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1488AC62-2553-41A1-BF66-2CB68340C396}">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1233,6 +1233,9 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>27</v>
+      </c>
       <c r="B29" t="s">
         <v>62</v>
       </c>
@@ -1253,6 +1256,9 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>28</v>
+      </c>
       <c r="B30" t="s">
         <v>62</v>
       </c>
@@ -1274,7 +1280,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B31" t="s">
         <v>62</v>
@@ -1295,7 +1301,7 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B32" t="s">
         <v>62</v>
@@ -1316,7 +1322,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B33" t="s">
         <v>62</v>
@@ -1337,7 +1343,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B34" t="s">
         <v>32</v>
@@ -1361,7 +1367,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B35" t="s">
         <v>32</v>
@@ -1385,7 +1391,7 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B36" t="s">
         <v>32</v>
@@ -1409,7 +1415,7 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B37" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
Added energyAsset javaclasses and instantiated
EnergyAssets now operate as instantiated abstract javaclasses that inherit more generic variables and functions, overriding for specific AssetTypes (windmill, photovoltaic, etc.).
-Default energyAssets for NetConnections are centrally added to the energyAsset-population in the main (now only J_EAOtherElectricityConsumption for houses, offices and buildings).
-EnergyAsset energy production and consumption are calculated and aggregated per netConnection and energy type.
-Started on the Conversion type energyAsset (J_EAGasBurner).
-Added model parameters for peak auxiliary electricity demand for houses, stores, offices. To be scaled with a normalized profile later.
</commit_message>
<xml_diff>
--- a/Base/db_backboneConfig.xlsx
+++ b/Base/db_backboneConfig.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\HOUJ\Documents\GitHub\HOLON\Base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E8D32AA-EE99-409D-8F25-1F7C25F05B31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDC04CD2-9BDB-49CD-8E2B-F71D106B9E6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C61B0771-0652-4F35-8DF1-D2D550B8F66D}"/>
   </bookViews>
@@ -583,7 +583,7 @@
   <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="O26" sqref="O26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Storage EnergyAsset, EnergyManager Agent, tijdreeksen
-EnergyManager agent en eerste functionaliteit toegevoegd
-Storage EnergyAsset en eerste functionaliteit toegevoegd
-Tijdreeksen voor genormaliseerde zonpv-opbrengst, ambient temperatuur toegevoegd.
</commit_message>
<xml_diff>
--- a/Base/db_backboneConfig.xlsx
+++ b/Base/db_backboneConfig.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\HOUJ\Documents\GitHub\HOLON\Base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDC04CD2-9BDB-49CD-8E2B-F71D106B9E6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0576B34-08E4-4562-B38A-A4AFCC40E6FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C61B0771-0652-4F35-8DF1-D2D550B8F66D}"/>
   </bookViews>
@@ -583,7 +583,7 @@
   <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="O26" sqref="O26"/>
+      <selection activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1434,8 +1434,7 @@
         <v>b27</v>
       </c>
       <c r="G37">
-        <f>300/1000*100</f>
-        <v>30</v>
+        <v>300</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Default energyAsset types addition
-Default energy assets are defined in an external database and may be added using option lists (parameter values are pre-defined)
-Option lists for energy asset types and default types
-Universal function for returning energy asset energyflows (werkt nog niet goed!)
-Backbone config by excelsheet is split up by agent type so optionlists can be used instead of string values
</commit_message>
<xml_diff>
--- a/Base/db_backboneConfig.xlsx
+++ b/Base/db_backboneConfig.xlsx
@@ -8,12 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\HOUJ\Documents\GitHub\HOLON\Base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3E249D5-5558-4549-81F0-9D92EA8C253C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{173581D3-53EC-43F9-9BD8-E050989E7B02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C61B0771-0652-4F35-8DF1-D2D550B8F66D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{C61B0771-0652-4F35-8DF1-D2D550B8F66D}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" r:id="rId1"/>
+    <sheet name="config_netNodes" sheetId="3" r:id="rId2"/>
+    <sheet name="config_netConnections" sheetId="2" r:id="rId3"/>
+    <sheet name="config_energyAssets" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="65">
   <si>
     <t>id</t>
   </si>
@@ -88,12 +91,6 @@
     <t>MSLS</t>
   </si>
   <si>
-    <t>MT4</t>
-  </si>
-  <si>
-    <t>building</t>
-  </si>
-  <si>
     <t>b1</t>
   </si>
   <si>
@@ -121,18 +118,6 @@
     <t>b9</t>
   </si>
   <si>
-    <t>house</t>
-  </si>
-  <si>
-    <t>detached</t>
-  </si>
-  <si>
-    <t>terraced</t>
-  </si>
-  <si>
-    <t>semidetached</t>
-  </si>
-  <si>
     <t>energyAsset</t>
   </si>
   <si>
@@ -145,27 +130,15 @@
     <t>a3</t>
   </si>
   <si>
-    <t>production</t>
-  </si>
-  <si>
     <t>b10</t>
   </si>
   <si>
     <t>b11</t>
   </si>
   <si>
-    <t>windfarm</t>
-  </si>
-  <si>
     <t>b12</t>
   </si>
   <si>
-    <t>solarfarm</t>
-  </si>
-  <si>
-    <t>store</t>
-  </si>
-  <si>
     <t>b13</t>
   </si>
   <si>
@@ -208,15 +181,6 @@
     <t>a4</t>
   </si>
   <si>
-    <t>windmill</t>
-  </si>
-  <si>
-    <t>solarpanel</t>
-  </si>
-  <si>
-    <t>office</t>
-  </si>
-  <si>
     <t>b26</t>
   </si>
   <si>
@@ -224,13 +188,58 @@
   </si>
   <si>
     <t>netConnection</t>
+  </si>
+  <si>
+    <t>PRODUCTION</t>
+  </si>
+  <si>
+    <t>WINDMILL</t>
+  </si>
+  <si>
+    <t>PHOTOVOLTAIC</t>
+  </si>
+  <si>
+    <t>MT</t>
+  </si>
+  <si>
+    <t>HOUSE</t>
+  </si>
+  <si>
+    <t>BUILDING</t>
+  </si>
+  <si>
+    <t>WINDFARM</t>
+  </si>
+  <si>
+    <t>SOLARFARM</t>
+  </si>
+  <si>
+    <t>DETACHED</t>
+  </si>
+  <si>
+    <t>TERRACED</t>
+  </si>
+  <si>
+    <t>SEMIDETACHED</t>
+  </si>
+  <si>
+    <t>STORE</t>
+  </si>
+  <si>
+    <t>OFFICE</t>
+  </si>
+  <si>
+    <t>a5</t>
+  </si>
+  <si>
+    <t>a6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="9"/>
       <color theme="1"/>
@@ -239,6 +248,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="9"/>
+      <color theme="1"/>
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
@@ -263,9 +279,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -580,10 +598,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1488AC62-2553-41A1-BF66-2CB68340C396}">
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -595,6 +613,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{243F788D-3AF5-439A-A91F-12D1BED9A308}">
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -697,7 +758,7 @@
         <v>8</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
       <c r="G5" s="1">
         <v>300000</v>
@@ -726,24 +787,181 @@
         <v>1000</v>
       </c>
     </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{493E8F37-4D53-4D4B-B589-A17DE4D133AF}">
+  <dimension ref="A1:G28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" t="s">
+        <v>60</v>
+      </c>
+      <c r="F4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="1">
+        <v>11</v>
+      </c>
+    </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D7" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="E7" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="F7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G7" s="1">
         <v>11</v>
@@ -754,19 +972,19 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D8" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="E8" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="F8" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G8" s="1">
         <v>11</v>
@@ -777,19 +995,19 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D9" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="E9" t="s">
-        <v>31</v>
+        <v>58</v>
       </c>
       <c r="F9" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G9" s="1">
         <v>11</v>
@@ -800,19 +1018,19 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D10" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="E10" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="F10" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G10" s="1">
         <v>11</v>
@@ -823,19 +1041,19 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D11" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="E11" t="s">
-        <v>31</v>
+        <v>58</v>
       </c>
       <c r="F11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G11" s="1">
         <v>11</v>
@@ -846,19 +1064,19 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="D12" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="E12" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="F12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G12" s="1">
         <v>11</v>
@@ -869,19 +1087,19 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="C13" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D13" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="E13" t="s">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="F13" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G13" s="1">
         <v>11</v>
@@ -892,19 +1110,19 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="C14" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="D14" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="E14" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="F14" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G14" s="1">
         <v>11</v>
@@ -915,19 +1133,19 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="C15" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="D15" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="E15" t="s">
-        <v>29</v>
+        <v>60</v>
       </c>
       <c r="F15" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G15" s="1">
         <v>11</v>
@@ -938,19 +1156,19 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="C16" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D16" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="E16" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="F16" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G16" s="1">
         <v>11</v>
@@ -961,19 +1179,19 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="C17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D17" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="E17" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="F17" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G17" s="1">
         <v>11</v>
@@ -984,19 +1202,19 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="C18" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D18" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="E18" t="s">
-        <v>31</v>
+        <v>58</v>
       </c>
       <c r="F18" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G18" s="1">
         <v>11</v>
@@ -1007,19 +1225,19 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="C19" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D19" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="E19" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="F19" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G19" s="1">
         <v>11</v>
@@ -1030,22 +1248,22 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="C20" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D20" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="E20" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="F20" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G20" s="1">
-        <v>11</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -1053,22 +1271,22 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="C21" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D21" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="E21" t="s">
-        <v>30</v>
+        <v>61</v>
       </c>
       <c r="F21" t="s">
         <v>4</v>
       </c>
       <c r="G21" s="1">
-        <v>11</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -1076,22 +1294,22 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="C22" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D22" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="E22" t="s">
-        <v>30</v>
+        <v>61</v>
       </c>
       <c r="F22" t="s">
         <v>6</v>
       </c>
       <c r="G22" s="1">
-        <v>11</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
@@ -1099,22 +1317,22 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="C23" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D23" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="E23" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
       <c r="F23" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G23" s="1">
-        <v>11</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -1122,22 +1340,22 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" t="s">
+        <v>43</v>
+      </c>
+      <c r="D24" t="s">
+        <v>55</v>
+      </c>
+      <c r="E24" t="s">
         <v>62</v>
       </c>
-      <c r="C24" t="s">
-        <v>48</v>
-      </c>
-      <c r="D24" t="s">
-        <v>28</v>
-      </c>
-      <c r="E24" t="s">
-        <v>29</v>
-      </c>
       <c r="F24" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G24" s="1">
-        <v>11</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -1145,19 +1363,19 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" t="s">
+        <v>44</v>
+      </c>
+      <c r="D25" t="s">
+        <v>55</v>
+      </c>
+      <c r="E25" t="s">
         <v>62</v>
       </c>
-      <c r="C25" t="s">
-        <v>49</v>
-      </c>
-      <c r="D25" t="s">
-        <v>18</v>
-      </c>
-      <c r="E25" t="s">
-        <v>42</v>
-      </c>
       <c r="F25" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G25" s="1">
         <v>50</v>
@@ -1168,22 +1386,20 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="C26" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D26" t="s">
-        <v>18</v>
-      </c>
-      <c r="E26" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="F26" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G26" s="1">
-        <v>50</v>
+        <f>400*1000</f>
+        <v>400000</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
@@ -1191,22 +1407,20 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="C27" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D27" t="s">
-        <v>18</v>
-      </c>
-      <c r="E27" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="F27" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G27" s="1">
-        <v>50</v>
+        <f>400*1000</f>
+        <v>400000</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -1214,231 +1428,205 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="C28" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D28" t="s">
-        <v>18</v>
-      </c>
-      <c r="E28" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="F28" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G28" s="1">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29">
-        <v>27</v>
-      </c>
-      <c r="B29" t="s">
-        <v>62</v>
-      </c>
-      <c r="C29" t="s">
-        <v>53</v>
-      </c>
-      <c r="D29" t="s">
-        <v>18</v>
-      </c>
-      <c r="E29" t="s">
-        <v>59</v>
-      </c>
-      <c r="F29" t="s">
-        <v>4</v>
-      </c>
-      <c r="G29" s="1">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30">
-        <v>28</v>
-      </c>
-      <c r="B30" t="s">
-        <v>62</v>
-      </c>
-      <c r="C30" t="s">
-        <v>54</v>
-      </c>
-      <c r="D30" t="s">
-        <v>18</v>
-      </c>
-      <c r="E30" t="s">
-        <v>59</v>
-      </c>
-      <c r="F30" t="s">
-        <v>6</v>
-      </c>
-      <c r="G30" s="1">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31">
-        <v>29</v>
-      </c>
-      <c r="B31" t="s">
-        <v>62</v>
-      </c>
-      <c r="C31" t="s">
-        <v>55</v>
-      </c>
-      <c r="D31" t="s">
-        <v>39</v>
-      </c>
-      <c r="F31" t="s">
-        <v>3</v>
-      </c>
-      <c r="G31" s="1">
         <f>400*1000</f>
         <v>400000</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32">
-        <v>30</v>
-      </c>
-      <c r="B32" t="s">
-        <v>62</v>
-      </c>
-      <c r="C32" t="s">
-        <v>60</v>
-      </c>
-      <c r="D32" t="s">
-        <v>39</v>
-      </c>
-      <c r="F32" t="s">
-        <v>4</v>
-      </c>
-      <c r="G32" s="1">
-        <f>400*1000</f>
-        <v>400000</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A33">
-        <v>31</v>
-      </c>
-      <c r="B33" t="s">
-        <v>62</v>
-      </c>
-      <c r="C33" t="s">
-        <v>61</v>
-      </c>
-      <c r="D33" t="s">
-        <v>41</v>
-      </c>
-      <c r="F33" t="s">
-        <v>6</v>
-      </c>
-      <c r="G33" s="1">
-        <f>400*1000</f>
-        <v>400000</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34">
-        <v>32</v>
-      </c>
-      <c r="B34" t="s">
-        <v>32</v>
-      </c>
-      <c r="C34" t="s">
-        <v>33</v>
-      </c>
-      <c r="D34" t="s">
-        <v>36</v>
-      </c>
-      <c r="E34" t="s">
-        <v>57</v>
-      </c>
-      <c r="F34" t="str">
-        <f>C31</f>
-        <v>b25</v>
-      </c>
-      <c r="G34" s="1">
-        <v>30000</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35">
-        <v>33</v>
-      </c>
-      <c r="B35" t="s">
-        <v>32</v>
-      </c>
-      <c r="C35" t="s">
-        <v>34</v>
-      </c>
-      <c r="D35" t="s">
-        <v>36</v>
-      </c>
-      <c r="E35" t="s">
-        <v>57</v>
-      </c>
-      <c r="F35" t="str">
-        <f>C32</f>
-        <v>b26</v>
-      </c>
-      <c r="G35" s="1">
-        <v>6000</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36">
-        <v>34</v>
-      </c>
-      <c r="B36" t="s">
-        <v>32</v>
-      </c>
-      <c r="C36" t="s">
-        <v>35</v>
-      </c>
-      <c r="D36" t="s">
-        <v>36</v>
-      </c>
-      <c r="E36" t="s">
-        <v>57</v>
-      </c>
-      <c r="F36" t="str">
-        <f>C32</f>
-        <v>b26</v>
-      </c>
-      <c r="G36" s="1">
-        <v>40000</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A37">
-        <v>35</v>
-      </c>
-      <c r="B37" t="s">
-        <v>32</v>
-      </c>
-      <c r="C37" t="s">
-        <v>56</v>
-      </c>
-      <c r="D37" t="s">
-        <v>36</v>
-      </c>
-      <c r="E37" t="s">
-        <v>58</v>
-      </c>
-      <c r="F37" t="str">
-        <f>C33</f>
-        <v>b27</v>
-      </c>
-      <c r="G37" s="1">
-        <v>300</v>
-      </c>
-    </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB486294-FB31-4C8F-BAEC-47B37B38DF9C}">
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="17.33203125" customWidth="1"/>
+    <col min="4" max="4" width="17" customWidth="1"/>
+    <col min="5" max="5" width="23.33203125" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" s="1">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G3" s="1">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G4" s="1">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G5" s="1">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
+        <v>64</v>
+      </c>
+      <c r="D7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" t="s">
+        <v>52</v>
+      </c>
+      <c r="F7" t="s">
+        <v>48</v>
+      </c>
+      <c r="G7" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
District heating network, default storage energy assets
-Heat nodes are initated
-District Heating netConnection agents connect to heat nodes
-House and building netConnection agents may connect to both an electrical node and a heat node.
-Default (preset) storage energy assets can be added to netConnection agents
-Default (preset) energy assets for district heating are added to the District Heating netConnection agent
</commit_message>
<xml_diff>
--- a/Base/db_backboneConfig.xlsx
+++ b/Base/db_backboneConfig.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\HOUJ\Documents\GitHub\HOLON\Base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{173581D3-53EC-43F9-9BD8-E050989E7B02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2D152A3-CB38-45AF-82CE-9D5F0DD03943}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{C61B0771-0652-4F35-8DF1-D2D550B8F66D}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="69">
   <si>
     <t>id</t>
   </si>
@@ -233,6 +233,18 @@
   </si>
   <si>
     <t>a6</t>
+  </si>
+  <si>
+    <t>DISTRICTHEATING</t>
+  </si>
+  <si>
+    <t>b28</t>
+  </si>
+  <si>
+    <t>parent_electric</t>
+  </si>
+  <si>
+    <t>parent_heat</t>
   </si>
 </sst>
 </file>
@@ -647,12 +659,13 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -794,19 +807,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{493E8F37-4D53-4D4B-B589-A17DE4D133AF}">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" customWidth="1"/>
+    <col min="6" max="6" width="14.1640625" customWidth="1"/>
+    <col min="7" max="7" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -823,13 +839,16 @@
         <v>14</v>
       </c>
       <c r="F1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -848,11 +867,11 @@
       <c r="F2" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="1">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -871,11 +890,11 @@
       <c r="F3" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="1">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H3" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -894,11 +913,14 @@
       <c r="F4" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="1">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -917,11 +939,11 @@
       <c r="F5" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="1">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H5" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -940,11 +962,11 @@
       <c r="F6" t="s">
         <v>4</v>
       </c>
-      <c r="G6" s="1">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H6" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -963,11 +985,11 @@
       <c r="F7" t="s">
         <v>4</v>
       </c>
-      <c r="G7" s="1">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H7" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -986,11 +1008,11 @@
       <c r="F8" t="s">
         <v>6</v>
       </c>
-      <c r="G8" s="1">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H8" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1009,11 +1031,11 @@
       <c r="F9" t="s">
         <v>6</v>
       </c>
-      <c r="G9" s="1">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H9" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1032,11 +1054,11 @@
       <c r="F10" t="s">
         <v>6</v>
       </c>
-      <c r="G10" s="1">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H10" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1055,11 +1077,14 @@
       <c r="F11" t="s">
         <v>3</v>
       </c>
-      <c r="G11" s="1">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G11" t="s">
+        <v>5</v>
+      </c>
+      <c r="H11" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1078,11 +1103,14 @@
       <c r="F12" t="s">
         <v>3</v>
       </c>
-      <c r="G12" s="1">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G12" t="s">
+        <v>5</v>
+      </c>
+      <c r="H12" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1101,11 +1129,14 @@
       <c r="F13" t="s">
         <v>3</v>
       </c>
-      <c r="G13" s="1">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G13" t="s">
+        <v>5</v>
+      </c>
+      <c r="H13" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1124,11 +1155,11 @@
       <c r="F14" t="s">
         <v>4</v>
       </c>
-      <c r="G14" s="1">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H14" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1147,11 +1178,11 @@
       <c r="F15" t="s">
         <v>4</v>
       </c>
-      <c r="G15" s="1">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H15" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1170,11 +1201,11 @@
       <c r="F16" t="s">
         <v>4</v>
       </c>
-      <c r="G16" s="1">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H16" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1193,11 +1224,11 @@
       <c r="F17" t="s">
         <v>6</v>
       </c>
-      <c r="G17" s="1">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H17" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1216,11 +1247,11 @@
       <c r="F18" t="s">
         <v>6</v>
       </c>
-      <c r="G18" s="1">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H18" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1239,11 +1270,11 @@
       <c r="F19" t="s">
         <v>6</v>
       </c>
-      <c r="G19" s="1">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H19" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1262,11 +1293,14 @@
       <c r="F20" t="s">
         <v>3</v>
       </c>
-      <c r="G20" s="1">
+      <c r="G20" t="s">
+        <v>5</v>
+      </c>
+      <c r="H20" s="1">
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1285,11 +1319,11 @@
       <c r="F21" t="s">
         <v>4</v>
       </c>
-      <c r="G21" s="1">
+      <c r="H21" s="1">
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1308,11 +1342,11 @@
       <c r="F22" t="s">
         <v>6</v>
       </c>
-      <c r="G22" s="1">
+      <c r="H22" s="1">
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>21</v>
       </c>
@@ -1331,11 +1365,11 @@
       <c r="F23" t="s">
         <v>3</v>
       </c>
-      <c r="G23" s="1">
+      <c r="H23" s="1">
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>22</v>
       </c>
@@ -1354,11 +1388,11 @@
       <c r="F24" t="s">
         <v>4</v>
       </c>
-      <c r="G24" s="1">
+      <c r="H24" s="1">
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>23</v>
       </c>
@@ -1377,11 +1411,11 @@
       <c r="F25" t="s">
         <v>6</v>
       </c>
-      <c r="G25" s="1">
+      <c r="H25" s="1">
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>24</v>
       </c>
@@ -1397,12 +1431,12 @@
       <c r="F26" t="s">
         <v>3</v>
       </c>
-      <c r="G26" s="1">
+      <c r="H26" s="1">
         <f>400*1000</f>
         <v>400000</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>25</v>
       </c>
@@ -1418,12 +1452,12 @@
       <c r="F27" t="s">
         <v>4</v>
       </c>
-      <c r="G27" s="1">
+      <c r="H27" s="1">
         <f>400*1000</f>
         <v>400000</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>26</v>
       </c>
@@ -1439,8 +1473,31 @@
       <c r="F28" t="s">
         <v>6</v>
       </c>
-      <c r="G28" s="1">
+      <c r="H28" s="1">
         <f>400*1000</f>
+        <v>400000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>49</v>
+      </c>
+      <c r="C29" t="s">
+        <v>66</v>
+      </c>
+      <c r="D29" t="s">
+        <v>65</v>
+      </c>
+      <c r="F29" t="s">
+        <v>3</v>
+      </c>
+      <c r="G29" t="s">
+        <v>5</v>
+      </c>
+      <c r="H29">
         <v>400000</v>
       </c>
     </row>
@@ -1454,7 +1511,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1582,7 +1639,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>26</v>
@@ -1605,7 +1662,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
Backbone energy assets, wind production profile
-Energy (production) assets from the backbone config file are again added to the model (windfarms, solarfarms),
-wind normalized profile is added based on ETM-script output,
-wind production assets use profile succesfully,
-first start on visualization of heat networks (districtheating netConnection agent works)
</commit_message>
<xml_diff>
--- a/Base/db_backboneConfig.xlsx
+++ b/Base/db_backboneConfig.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\HOUJ\Documents\GitHub\HOLON\Base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2D152A3-CB38-45AF-82CE-9D5F0DD03943}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEB79E53-C010-46BF-94E2-CAB96D0226D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{C61B0771-0652-4F35-8DF1-D2D550B8F66D}"/>
+    <workbookView xWindow="2250" yWindow="2250" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{C61B0771-0652-4F35-8DF1-D2D550B8F66D}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="71">
   <si>
     <t>id</t>
   </si>
@@ -245,6 +245,12 @@
   </si>
   <si>
     <t>parent_heat</t>
+  </si>
+  <si>
+    <t>capacity_electric_kw</t>
+  </si>
+  <si>
+    <t>capacity_heat_kw</t>
   </si>
 </sst>
 </file>
@@ -1508,10 +1514,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB486294-FB31-4C8F-BAEC-47B37B38DF9C}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1522,7 +1528,7 @@
     <col min="6" max="6" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -1542,10 +1548,13 @@
         <v>11</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+      <c r="H1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1567,8 +1576,11 @@
       <c r="G2" s="1">
         <v>3000</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1590,8 +1602,11 @@
       <c r="G3" s="1">
         <v>5000</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1613,8 +1628,11 @@
       <c r="G4" s="1">
         <v>5000</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1636,8 +1654,11 @@
       <c r="G5" s="1">
         <v>3000</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1659,8 +1680,11 @@
       <c r="G6" s="1">
         <v>1000</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1681,6 +1705,9 @@
       </c>
       <c r="G7" s="1">
         <v>1000</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Heat net node visualisation, heat delivery set
-Heat nodes and their connections are visualized in the KPIVisuals agent
-NetNode energy calculations now include all energy carriers (todo: make flows conditional on connection type),
-Heat delivery set is added as a default energyAsset and abstract class
</commit_message>
<xml_diff>
--- a/Base/db_backboneConfig.xlsx
+++ b/Base/db_backboneConfig.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\HOUJ\Documents\GitHub\HOLON\Base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEB79E53-C010-46BF-94E2-CAB96D0226D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64738793-FEEF-424E-9A1C-7ACD605D92CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2250" yWindow="2250" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{C61B0771-0652-4F35-8DF1-D2D550B8F66D}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{C61B0771-0652-4F35-8DF1-D2D550B8F66D}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" r:id="rId1"/>
@@ -665,7 +665,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -815,8 +815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{493E8F37-4D53-4D4B-B589-A17DE4D133AF}">
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1435,7 +1435,7 @@
         <v>56</v>
       </c>
       <c r="F26" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H26" s="1">
         <f>400*1000</f>
@@ -1456,7 +1456,7 @@
         <v>56</v>
       </c>
       <c r="F27" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H27" s="1">
         <f>400*1000</f>
@@ -1477,7 +1477,7 @@
         <v>57</v>
       </c>
       <c r="F28" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="H28" s="1">
         <f>400*1000</f>
@@ -1516,8 +1516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB486294-FB31-4C8F-BAEC-47B37B38DF9C}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
heat delivery set allocation, energy flow updates
-(only) houses with heat connection get a heat delivery set energyAsset so energy flows are explicitly accounted
-energy flows in NetConnections and NetNodes are only listed if <> zero to save memory space.
-Separate calculation and operation of district heating type netconnections to enable determination of energy balance in heat net.
</commit_message>
<xml_diff>
--- a/Base/db_backboneConfig.xlsx
+++ b/Base/db_backboneConfig.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\HOUJ\Documents\GitHub\HOLON\Base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64738793-FEEF-424E-9A1C-7ACD605D92CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7C1030D-B964-4F79-BF5A-9D57E0C57628}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{C61B0771-0652-4F35-8DF1-D2D550B8F66D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{C61B0771-0652-4F35-8DF1-D2D550B8F66D}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" r:id="rId1"/>
@@ -815,8 +815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{493E8F37-4D53-4D4B-B589-A17DE4D133AF}">
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Added actor agents and connected them to NetConnections and each other
No functionality yet, besides creating agents and making agent-connections
</commit_message>
<xml_diff>
--- a/Base/db_backboneConfig.xlsx
+++ b/Base/db_backboneConfig.xlsx
@@ -5,18 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\HOUJ\Documents\GitHub\HOLON\Base\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gilli\Documents\Project HOLON\Git_Local_Clone\HOLON\Base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7C1030D-B964-4F79-BF5A-9D57E0C57628}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{624A81B3-DC45-4979-84B2-6CC1A966A674}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{C61B0771-0652-4F35-8DF1-D2D550B8F66D}"/>
+    <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="2" xr2:uid="{C61B0771-0652-4F35-8DF1-D2D550B8F66D}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" r:id="rId1"/>
     <sheet name="config_netNodes" sheetId="3" r:id="rId2"/>
     <sheet name="config_netConnections" sheetId="2" r:id="rId3"/>
-    <sheet name="config_energyAssets" sheetId="4" r:id="rId4"/>
+    <sheet name="config_actors" sheetId="5" r:id="rId4"/>
+    <sheet name="config_energyAssets" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="106">
   <si>
     <t>id</t>
   </si>
@@ -251,6 +252,111 @@
   </si>
   <si>
     <t>capacity_heat_kw</t>
+  </si>
+  <si>
+    <t>actortype</t>
+  </si>
+  <si>
+    <t>household</t>
+  </si>
+  <si>
+    <t>hh1</t>
+  </si>
+  <si>
+    <t>hh2</t>
+  </si>
+  <si>
+    <t>hh3</t>
+  </si>
+  <si>
+    <t>hh4</t>
+  </si>
+  <si>
+    <t>hh5</t>
+  </si>
+  <si>
+    <t>hh6</t>
+  </si>
+  <si>
+    <t>hh7</t>
+  </si>
+  <si>
+    <t>hh8</t>
+  </si>
+  <si>
+    <t>hh9</t>
+  </si>
+  <si>
+    <t>hh10</t>
+  </si>
+  <si>
+    <t>hh11</t>
+  </si>
+  <si>
+    <t>hh12</t>
+  </si>
+  <si>
+    <t>hh13</t>
+  </si>
+  <si>
+    <t>hh14</t>
+  </si>
+  <si>
+    <t>hh15</t>
+  </si>
+  <si>
+    <t>hh16</t>
+  </si>
+  <si>
+    <t>hh17</t>
+  </si>
+  <si>
+    <t>hh18</t>
+  </si>
+  <si>
+    <t>parent_actor</t>
+  </si>
+  <si>
+    <t>owner_actor</t>
+  </si>
+  <si>
+    <t>com1</t>
+  </si>
+  <si>
+    <t>com2</t>
+  </si>
+  <si>
+    <t>sup1</t>
+  </si>
+  <si>
+    <t>sup2</t>
+  </si>
+  <si>
+    <t>commercial</t>
+  </si>
+  <si>
+    <t>energysupplier</t>
+  </si>
+  <si>
+    <t>holon</t>
+  </si>
+  <si>
+    <t>hol1</t>
+  </si>
+  <si>
+    <t>nat</t>
+  </si>
+  <si>
+    <t>HOUSEHOLD</t>
+  </si>
+  <si>
+    <t>COMMERCIAL</t>
+  </si>
+  <si>
+    <t>ENERGYSUPPLIER</t>
+  </si>
+  <si>
+    <t>HOLON</t>
   </si>
 </sst>
 </file>
@@ -813,10 +919,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{493E8F37-4D53-4D4B-B589-A17DE4D133AF}">
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N24" sqref="N24"/>
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -828,7 +934,7 @@
     <col min="7" max="7" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -853,8 +959,11 @@
       <c r="H1" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -876,8 +985,11 @@
       <c r="H2" s="1">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -899,8 +1011,11 @@
       <c r="H3" s="1">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -925,8 +1040,11 @@
       <c r="H4" s="1">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -948,8 +1066,11 @@
       <c r="H5" s="1">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -971,8 +1092,11 @@
       <c r="H6" s="1">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -994,8 +1118,11 @@
       <c r="H7" s="1">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1017,8 +1144,11 @@
       <c r="H8" s="1">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1040,8 +1170,11 @@
       <c r="H9" s="1">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1063,8 +1196,11 @@
       <c r="H10" s="1">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1089,8 +1225,11 @@
       <c r="H11" s="1">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1115,8 +1254,11 @@
       <c r="H12" s="1">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I12" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1141,8 +1283,11 @@
       <c r="H13" s="1">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I13" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1164,8 +1309,11 @@
       <c r="H14" s="1">
         <v>11</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I14" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1187,8 +1335,11 @@
       <c r="H15" s="1">
         <v>11</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I15" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1210,8 +1361,11 @@
       <c r="H16" s="1">
         <v>11</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I16" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1233,8 +1387,11 @@
       <c r="H17" s="1">
         <v>11</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I17" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1256,8 +1413,11 @@
       <c r="H18" s="1">
         <v>11</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I18" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1279,8 +1439,11 @@
       <c r="H19" s="1">
         <v>11</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I19" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1305,8 +1468,11 @@
       <c r="H20" s="1">
         <v>50</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I20" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1328,8 +1494,11 @@
       <c r="H21" s="1">
         <v>50</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I21" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1351,8 +1520,11 @@
       <c r="H22" s="1">
         <v>50</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I22" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>21</v>
       </c>
@@ -1374,8 +1546,11 @@
       <c r="H23" s="1">
         <v>50</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I23" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>22</v>
       </c>
@@ -1397,8 +1572,11 @@
       <c r="H24" s="1">
         <v>50</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I24" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>23</v>
       </c>
@@ -1420,8 +1598,11 @@
       <c r="H25" s="1">
         <v>50</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I25" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>24</v>
       </c>
@@ -1441,8 +1622,11 @@
         <f>400*1000</f>
         <v>400000</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I26" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>25</v>
       </c>
@@ -1462,8 +1646,11 @@
         <f>400*1000</f>
         <v>400000</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I27" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>26</v>
       </c>
@@ -1483,8 +1670,11 @@
         <f>400*1000</f>
         <v>400000</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I28" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>27</v>
       </c>
@@ -1505,6 +1695,9 @@
       </c>
       <c r="H29">
         <v>400000</v>
+      </c>
+      <c r="I29" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1513,6 +1706,434 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F595F011-BCBA-42A0-B2C1-EC2B9C01AA0D}">
+  <dimension ref="A1:E24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="3" width="19.33203125" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D6" t="s">
+        <v>77</v>
+      </c>
+      <c r="E6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" t="s">
+        <v>102</v>
+      </c>
+      <c r="D7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8" t="s">
+        <v>102</v>
+      </c>
+      <c r="D8" t="s">
+        <v>79</v>
+      </c>
+      <c r="E8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" t="s">
+        <v>102</v>
+      </c>
+      <c r="D9" t="s">
+        <v>80</v>
+      </c>
+      <c r="E9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10" t="s">
+        <v>102</v>
+      </c>
+      <c r="D10" t="s">
+        <v>81</v>
+      </c>
+      <c r="E10" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>72</v>
+      </c>
+      <c r="C11" t="s">
+        <v>102</v>
+      </c>
+      <c r="D11" t="s">
+        <v>82</v>
+      </c>
+      <c r="E11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" t="s">
+        <v>102</v>
+      </c>
+      <c r="D12" t="s">
+        <v>83</v>
+      </c>
+      <c r="E12" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>72</v>
+      </c>
+      <c r="C13" t="s">
+        <v>102</v>
+      </c>
+      <c r="D13" t="s">
+        <v>84</v>
+      </c>
+      <c r="E13" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>72</v>
+      </c>
+      <c r="C14" t="s">
+        <v>102</v>
+      </c>
+      <c r="D14" t="s">
+        <v>85</v>
+      </c>
+      <c r="E14" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>72</v>
+      </c>
+      <c r="C15" t="s">
+        <v>102</v>
+      </c>
+      <c r="D15" t="s">
+        <v>86</v>
+      </c>
+      <c r="E15" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>72</v>
+      </c>
+      <c r="C16" t="s">
+        <v>102</v>
+      </c>
+      <c r="D16" t="s">
+        <v>87</v>
+      </c>
+      <c r="E16" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>72</v>
+      </c>
+      <c r="C17" t="s">
+        <v>102</v>
+      </c>
+      <c r="D17" t="s">
+        <v>88</v>
+      </c>
+      <c r="E17" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>72</v>
+      </c>
+      <c r="C18" t="s">
+        <v>102</v>
+      </c>
+      <c r="D18" t="s">
+        <v>89</v>
+      </c>
+      <c r="E18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>72</v>
+      </c>
+      <c r="C19" t="s">
+        <v>102</v>
+      </c>
+      <c r="D19" t="s">
+        <v>90</v>
+      </c>
+      <c r="E19" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>97</v>
+      </c>
+      <c r="C20" t="s">
+        <v>103</v>
+      </c>
+      <c r="D20" t="s">
+        <v>93</v>
+      </c>
+      <c r="E20" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>97</v>
+      </c>
+      <c r="C21" t="s">
+        <v>103</v>
+      </c>
+      <c r="D21" t="s">
+        <v>94</v>
+      </c>
+      <c r="E21" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>98</v>
+      </c>
+      <c r="C22" t="s">
+        <v>104</v>
+      </c>
+      <c r="D22" t="s">
+        <v>95</v>
+      </c>
+      <c r="E22" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>98</v>
+      </c>
+      <c r="C23" t="s">
+        <v>104</v>
+      </c>
+      <c r="D23" t="s">
+        <v>96</v>
+      </c>
+      <c r="E23" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C24" t="s">
+        <v>105</v>
+      </c>
+      <c r="D24" t="s">
+        <v>100</v>
+      </c>
+      <c r="E24" t="s">
+        <v>101</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB486294-FB31-4C8F-BAEC-47B37B38DF9C}">
   <dimension ref="A1:H7"/>
   <sheetViews>

</xml_diff>

<commit_message>
Begin van twee visualisatiemodes voor actors in KPIVisuals
-Actors kunnen nu worden gevisualiseerd op twee manieren:
-individuele actoren en hun verbindingen met parent-actors,
-geaggregeerd in typen actoren met aantallen in beeld.
</commit_message>
<xml_diff>
--- a/Base/db_backboneConfig.xlsx
+++ b/Base/db_backboneConfig.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gilli\Documents\Project HOLON\Git_Local_Clone\HOLON\Base\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\HOUJ\Documents\GitHub\HOLON\Base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{624A81B3-DC45-4979-84B2-6CC1A966A674}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B0A4408-FFB7-47EB-A15E-3CDF852A08F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="2" xr2:uid="{C61B0771-0652-4F35-8DF1-D2D550B8F66D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{C61B0771-0652-4F35-8DF1-D2D550B8F66D}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="108">
   <si>
     <t>id</t>
   </si>
@@ -357,6 +357,12 @@
   </si>
   <si>
     <t>HOLON</t>
+  </si>
+  <si>
+    <t>com3</t>
+  </si>
+  <si>
+    <t>com4</t>
   </si>
 </sst>
 </file>
@@ -921,8 +927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{493E8F37-4D53-4D4B-B589-A17DE4D133AF}">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1495,7 +1501,7 @@
         <v>50</v>
       </c>
       <c r="I21" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
@@ -1521,7 +1527,7 @@
         <v>50</v>
       </c>
       <c r="I22" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
@@ -1547,7 +1553,7 @@
         <v>50</v>
       </c>
       <c r="I23" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
@@ -1573,7 +1579,7 @@
         <v>50</v>
       </c>
       <c r="I24" t="s">
-        <v>94</v>
+        <v>107</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
@@ -1599,7 +1605,7 @@
         <v>50</v>
       </c>
       <c r="I25" t="s">
-        <v>94</v>
+        <v>107</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
@@ -1709,8 +1715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F595F011-BCBA-42A0-B2C1-EC2B9C01AA0D}">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Fill populations of connectionOwners, energySuppliers and energyHolons
modified old actor-instantiation loop to instantiate the new different actor types. (placeholder until we update the database to the new structure)
</commit_message>
<xml_diff>
--- a/Base/db_backboneConfig.xlsx
+++ b/Base/db_backboneConfig.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\HOUJ\Documents\GitHub\HOLON\Base\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gilli\Documents\Project HOLON\Git_Local_Clone\HOLON\Base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B0A4408-FFB7-47EB-A15E-3CDF852A08F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{179A2A8A-9952-44EC-9F51-3FD69574229B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{C61B0771-0652-4F35-8DF1-D2D550B8F66D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" activeTab="3" xr2:uid="{C61B0771-0652-4F35-8DF1-D2D550B8F66D}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="107">
   <si>
     <t>id</t>
   </si>
@@ -347,22 +347,19 @@
     <t>nat</t>
   </si>
   <si>
-    <t>HOUSEHOLD</t>
-  </si>
-  <si>
-    <t>COMMERCIAL</t>
-  </si>
-  <si>
     <t>ENERGYSUPPLIER</t>
   </si>
   <si>
-    <t>HOLON</t>
-  </si>
-  <si>
     <t>com3</t>
   </si>
   <si>
     <t>com4</t>
+  </si>
+  <si>
+    <t>CONNECTIONOWNER</t>
+  </si>
+  <si>
+    <t>ENERGYHOLON</t>
   </si>
 </sst>
 </file>
@@ -1527,7 +1524,7 @@
         <v>50</v>
       </c>
       <c r="I22" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
@@ -1553,7 +1550,7 @@
         <v>50</v>
       </c>
       <c r="I23" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
@@ -1579,7 +1576,7 @@
         <v>50</v>
       </c>
       <c r="I24" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
@@ -1605,7 +1602,7 @@
         <v>50</v>
       </c>
       <c r="I25" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
@@ -1716,7 +1713,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1730,10 +1727,10 @@
         <v>12</v>
       </c>
       <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
         <v>71</v>
-      </c>
-      <c r="C1" t="s">
-        <v>9</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -1750,7 +1747,7 @@
         <v>72</v>
       </c>
       <c r="C2" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="D2" t="s">
         <v>73</v>
@@ -1767,7 +1764,7 @@
         <v>72</v>
       </c>
       <c r="C3" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="D3" t="s">
         <v>74</v>
@@ -1784,7 +1781,7 @@
         <v>72</v>
       </c>
       <c r="C4" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="D4" t="s">
         <v>75</v>
@@ -1801,7 +1798,7 @@
         <v>72</v>
       </c>
       <c r="C5" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="D5" t="s">
         <v>76</v>
@@ -1818,7 +1815,7 @@
         <v>72</v>
       </c>
       <c r="C6" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="D6" t="s">
         <v>77</v>
@@ -1835,7 +1832,7 @@
         <v>72</v>
       </c>
       <c r="C7" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="D7" t="s">
         <v>78</v>
@@ -1852,7 +1849,7 @@
         <v>72</v>
       </c>
       <c r="C8" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="D8" t="s">
         <v>79</v>
@@ -1869,7 +1866,7 @@
         <v>72</v>
       </c>
       <c r="C9" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="D9" t="s">
         <v>80</v>
@@ -1886,7 +1883,7 @@
         <v>72</v>
       </c>
       <c r="C10" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="D10" t="s">
         <v>81</v>
@@ -1903,7 +1900,7 @@
         <v>72</v>
       </c>
       <c r="C11" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="D11" t="s">
         <v>82</v>
@@ -1920,7 +1917,7 @@
         <v>72</v>
       </c>
       <c r="C12" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="D12" t="s">
         <v>83</v>
@@ -1937,7 +1934,7 @@
         <v>72</v>
       </c>
       <c r="C13" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="D13" t="s">
         <v>84</v>
@@ -1954,7 +1951,7 @@
         <v>72</v>
       </c>
       <c r="C14" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="D14" t="s">
         <v>85</v>
@@ -1971,7 +1968,7 @@
         <v>72</v>
       </c>
       <c r="C15" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="D15" t="s">
         <v>86</v>
@@ -1988,7 +1985,7 @@
         <v>72</v>
       </c>
       <c r="C16" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="D16" t="s">
         <v>87</v>
@@ -2005,7 +2002,7 @@
         <v>72</v>
       </c>
       <c r="C17" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="D17" t="s">
         <v>88</v>
@@ -2022,7 +2019,7 @@
         <v>72</v>
       </c>
       <c r="C18" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="D18" t="s">
         <v>89</v>
@@ -2039,7 +2036,7 @@
         <v>72</v>
       </c>
       <c r="C19" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="D19" t="s">
         <v>90</v>
@@ -2056,7 +2053,7 @@
         <v>97</v>
       </c>
       <c r="C20" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D20" t="s">
         <v>93</v>
@@ -2073,7 +2070,7 @@
         <v>97</v>
       </c>
       <c r="C21" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D21" t="s">
         <v>94</v>
@@ -2090,7 +2087,7 @@
         <v>98</v>
       </c>
       <c r="C22" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D22" t="s">
         <v>95</v>
@@ -2107,7 +2104,7 @@
         <v>98</v>
       </c>
       <c r="C23" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D23" t="s">
         <v>96</v>
@@ -2124,7 +2121,7 @@
         <v>99</v>
       </c>
       <c r="C24" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D24" t="s">
         <v>100</v>

</xml_diff>

<commit_message>
Passthrough-functionality for energyTransactions added to EnergyHolon agent
Now a ConnectionOwner can have an EnergyHolon as p_energySupplier
</commit_message>
<xml_diff>
--- a/Base/db_backboneConfig.xlsx
+++ b/Base/db_backboneConfig.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gilli\Documents\Project HOLON\Git_Local_Clone\HOLON\Base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{179A2A8A-9952-44EC-9F51-3FD69574229B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{634F3A5C-77BE-44BC-8062-75B202FDFC4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" activeTab="3" xr2:uid="{C61B0771-0652-4F35-8DF1-D2D550B8F66D}"/>
+    <workbookView xWindow="6780" yWindow="1710" windowWidth="38700" windowHeight="15375" activeTab="3" xr2:uid="{C61B0771-0652-4F35-8DF1-D2D550B8F66D}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="106">
   <si>
     <t>id</t>
   </si>
@@ -252,9 +252,6 @@
   </si>
   <si>
     <t>capacity_heat_kw</t>
-  </si>
-  <si>
-    <t>actortype</t>
   </si>
   <si>
     <t>household</t>
@@ -963,7 +960,7 @@
         <v>13</v>
       </c>
       <c r="I1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -989,7 +986,7 @@
         <v>11</v>
       </c>
       <c r="I2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -1015,7 +1012,7 @@
         <v>11</v>
       </c>
       <c r="I3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -1044,7 +1041,7 @@
         <v>11</v>
       </c>
       <c r="I4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -1070,7 +1067,7 @@
         <v>11</v>
       </c>
       <c r="I5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -1096,7 +1093,7 @@
         <v>11</v>
       </c>
       <c r="I6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -1122,7 +1119,7 @@
         <v>11</v>
       </c>
       <c r="I7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -1148,7 +1145,7 @@
         <v>11</v>
       </c>
       <c r="I8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -1174,7 +1171,7 @@
         <v>11</v>
       </c>
       <c r="I9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -1200,7 +1197,7 @@
         <v>11</v>
       </c>
       <c r="I10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -1229,7 +1226,7 @@
         <v>11</v>
       </c>
       <c r="I11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -1258,7 +1255,7 @@
         <v>11</v>
       </c>
       <c r="I12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -1287,7 +1284,7 @@
         <v>11</v>
       </c>
       <c r="I13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -1313,7 +1310,7 @@
         <v>11</v>
       </c>
       <c r="I14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -1339,7 +1336,7 @@
         <v>11</v>
       </c>
       <c r="I15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
@@ -1365,7 +1362,7 @@
         <v>11</v>
       </c>
       <c r="I16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
@@ -1391,7 +1388,7 @@
         <v>11</v>
       </c>
       <c r="I17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
@@ -1417,7 +1414,7 @@
         <v>11</v>
       </c>
       <c r="I18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
@@ -1443,7 +1440,7 @@
         <v>11</v>
       </c>
       <c r="I19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
@@ -1472,7 +1469,7 @@
         <v>50</v>
       </c>
       <c r="I20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
@@ -1498,7 +1495,7 @@
         <v>50</v>
       </c>
       <c r="I21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
@@ -1524,7 +1521,7 @@
         <v>50</v>
       </c>
       <c r="I22" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
@@ -1550,7 +1547,7 @@
         <v>50</v>
       </c>
       <c r="I23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
@@ -1576,7 +1573,7 @@
         <v>50</v>
       </c>
       <c r="I24" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
@@ -1602,7 +1599,7 @@
         <v>50</v>
       </c>
       <c r="I25" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
@@ -1626,7 +1623,7 @@
         <v>400000</v>
       </c>
       <c r="I26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
@@ -1650,7 +1647,7 @@
         <v>400000</v>
       </c>
       <c r="I27" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
@@ -1674,7 +1671,7 @@
         <v>400000</v>
       </c>
       <c r="I28" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
@@ -1700,7 +1697,7 @@
         <v>400000</v>
       </c>
       <c r="I29" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1713,7 +1710,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1730,13 +1727,13 @@
         <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>71</v>
+        <v>10</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1744,16 +1741,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D2" t="s">
         <v>72</v>
       </c>
-      <c r="C2" t="s">
-        <v>105</v>
-      </c>
-      <c r="D2" t="s">
-        <v>73</v>
-      </c>
       <c r="E2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -1761,16 +1758,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -1778,16 +1775,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -1795,16 +1792,16 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -1812,16 +1809,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -1829,16 +1826,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -1846,16 +1843,16 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -1863,16 +1860,16 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -1880,16 +1877,16 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -1897,16 +1894,16 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -1914,16 +1911,16 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -1931,16 +1928,16 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -1948,16 +1945,16 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C14" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -1965,16 +1962,16 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C15" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -1982,16 +1979,16 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C16" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -1999,16 +1996,16 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -2016,16 +2013,16 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -2033,16 +2030,16 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C19" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -2050,16 +2047,16 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E20" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -2067,16 +2064,16 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C21" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D21" t="s">
+        <v>93</v>
+      </c>
+      <c r="E21" t="s">
         <v>94</v>
-      </c>
-      <c r="E21" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -2084,16 +2081,16 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C22" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D22" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E22" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -2101,16 +2098,16 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D23" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E23" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -2118,16 +2115,16 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
+        <v>98</v>
+      </c>
+      <c r="C24" t="s">
+        <v>105</v>
+      </c>
+      <c r="D24" t="s">
         <v>99</v>
       </c>
-      <c r="C24" t="s">
-        <v>106</v>
-      </c>
-      <c r="D24" t="s">
-        <v>100</v>
-      </c>
       <c r="E24" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed execution order of MS and HS GridNode energyBalance
EnergyBalances need to be calculated 'bottom up' on the grid to have consistent numbers within a timestep. Execution order of the nodes is at the moment defined by the config excell, so to ensure the correct execution order the excell is edited.
</commit_message>
<xml_diff>
--- a/Base/db_backboneConfig.xlsx
+++ b/Base/db_backboneConfig.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gilli\Documents\Project HOLON\Git_Local_Clone\HOLON\Base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{634F3A5C-77BE-44BC-8062-75B202FDFC4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69D610DF-DBE5-42F8-9D72-C65BE5421849}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6780" yWindow="1710" windowWidth="38700" windowHeight="15375" activeTab="3" xr2:uid="{C61B0771-0652-4F35-8DF1-D2D550B8F66D}"/>
+    <workbookView xWindow="11430" yWindow="2040" windowWidth="38700" windowHeight="15375" activeTab="1" xr2:uid="{C61B0771-0652-4F35-8DF1-D2D550B8F66D}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" r:id="rId1"/>
@@ -770,8 +770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{243F788D-3AF5-439A-A91F-12D1BED9A308}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -811,16 +811,19 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>2</v>
       </c>
       <c r="G2" s="1">
-        <v>500000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -831,7 +834,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D3" t="s">
         <v>7</v>
@@ -854,7 +857,7 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
@@ -877,16 +880,16 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="G5" s="1">
-        <v>300000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -897,19 +900,16 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" t="s">
-        <v>2</v>
+        <v>53</v>
       </c>
       <c r="G6" s="1">
-        <v>1000</v>
+        <v>300000</v>
       </c>
     </row>
   </sheetData>
@@ -1709,7 +1709,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F595F011-BCBA-42A0-B2C1-EC2B9C01AA0D}">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fix for GridNode connections, system check variables
-GridNodes now connect to superior node again independent of the order of their creation.
-Added system consistency check variables in KpiVisuals
</commit_message>
<xml_diff>
--- a/Base/db_backboneConfig.xlsx
+++ b/Base/db_backboneConfig.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gilli\Documents\Project HOLON\Git_Local_Clone\HOLON\Base\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\HOUJ\Documents\GitHub\HOLON\Base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69D610DF-DBE5-42F8-9D72-C65BE5421849}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAA7863D-AD78-4F65-8547-8F62D644684D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11430" yWindow="2040" windowWidth="38700" windowHeight="15375" activeTab="1" xr2:uid="{C61B0771-0652-4F35-8DF1-D2D550B8F66D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{C61B0771-0652-4F35-8DF1-D2D550B8F66D}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" r:id="rId1"/>
@@ -770,8 +770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{243F788D-3AF5-439A-A91F-12D1BED9A308}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -921,8 +921,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{493E8F37-4D53-4D4B-B589-A17DE4D133AF}">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N27" sqref="N27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1616,7 +1616,7 @@
         <v>56</v>
       </c>
       <c r="F26" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H26" s="1">
         <f>400*1000</f>
@@ -1640,7 +1640,7 @@
         <v>56</v>
       </c>
       <c r="F27" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H27" s="1">
         <f>400*1000</f>
@@ -1664,7 +1664,7 @@
         <v>57</v>
       </c>
       <c r="F28" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H28" s="1">
         <f>400*1000</f>

</xml_diff>

<commit_message>
Dedicated energySupplier and accounting for district heating
**ConnectionOwners with district heated GridConnections now connect to the dedicated energy supplier for accounting of heat flows
**heat flows are accounted seperately, with the dedicated energy supplier (for ConnectionOwners with a district heating supplier)
**Note: District heating energy supplier is determined in-model (as the OwnerAgent of the DistrictHeating GridConnection-Agent). This works as long as there is only one such agent per DH-network!
</commit_message>
<xml_diff>
--- a/Base/db_backboneConfig.xlsx
+++ b/Base/db_backboneConfig.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\HOUJ\Documents\GitHub\HOLON\Base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAA7863D-AD78-4F65-8547-8F62D644684D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C9D1A84-4A7C-4512-B014-FFC3DB6ADD71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{C61B0771-0652-4F35-8DF1-D2D550B8F66D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{C61B0771-0652-4F35-8DF1-D2D550B8F66D}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" r:id="rId1"/>
@@ -770,8 +770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{243F788D-3AF5-439A-A91F-12D1BED9A308}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -921,8 +921,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{493E8F37-4D53-4D4B-B589-A17DE4D133AF}">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
GridConnections from JSON-data, fixes pythonscript
*GridConnections are now succesfully configured from JSON-string
*python-script for generating JSON-strings from db_backboneConfig.xlsx Excelsworkbook improved to use relative paths
</commit_message>
<xml_diff>
--- a/Base/db_backboneConfig.xlsx
+++ b/Base/db_backboneConfig.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\HOUJ\Documents\GitHub\HOLON\Base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C9D1A84-4A7C-4512-B014-FFC3DB6ADD71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B41B2986-4F76-4C7A-BDCD-2DDB2761F10C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{C61B0771-0652-4F35-8DF1-D2D550B8F66D}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{C61B0771-0652-4F35-8DF1-D2D550B8F66D}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="107">
   <si>
     <t>id</t>
   </si>
@@ -357,6 +357,9 @@
   </si>
   <si>
     <t>ENERGYHOLON</t>
+  </si>
+  <si>
+    <t>NONE</t>
   </si>
 </sst>
 </file>
@@ -770,7 +773,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{243F788D-3AF5-439A-A91F-12D1BED9A308}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
@@ -921,8 +924,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{493E8F37-4D53-4D4B-B589-A17DE4D133AF}">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1615,6 +1618,9 @@
       <c r="D26" t="s">
         <v>56</v>
       </c>
+      <c r="E26" t="s">
+        <v>106</v>
+      </c>
       <c r="F26" t="s">
         <v>3</v>
       </c>
@@ -1639,6 +1645,9 @@
       <c r="D27" t="s">
         <v>56</v>
       </c>
+      <c r="E27" t="s">
+        <v>106</v>
+      </c>
       <c r="F27" t="s">
         <v>4</v>
       </c>
@@ -1663,6 +1672,9 @@
       <c r="D28" t="s">
         <v>57</v>
       </c>
+      <c r="E28" t="s">
+        <v>106</v>
+      </c>
       <c r="F28" t="s">
         <v>6</v>
       </c>
@@ -1686,6 +1698,9 @@
       </c>
       <c r="D29" t="s">
         <v>65</v>
+      </c>
+      <c r="E29" t="s">
+        <v>106</v>
       </c>
       <c r="F29" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
Fixes config-excel, experiments for 27 and 300 agents
*sheetnames in de excel zijn nu consistent met de terminologie in het model (bijv. gridNode ipv netNode)
*python-scripts aangepast m.b.t. nieuwe sheetnames
*excelsheets met 27 en 300 agents, omgezet in jsons voor inladen in Anylogic met de text-objecten
</commit_message>
<xml_diff>
--- a/Base/db_backboneConfig.xlsx
+++ b/Base/db_backboneConfig.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\HOUJ\Documents\GitHub\HOLON\Base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B41B2986-4F76-4C7A-BDCD-2DDB2761F10C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57E639A8-DCDE-4E24-BA47-28B92801AE39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{C61B0771-0652-4F35-8DF1-D2D550B8F66D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{C61B0771-0652-4F35-8DF1-D2D550B8F66D}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" r:id="rId1"/>
-    <sheet name="config_netNodes" sheetId="3" r:id="rId2"/>
-    <sheet name="config_netConnections" sheetId="2" r:id="rId3"/>
+    <sheet name="config_gridNodes" sheetId="3" r:id="rId2"/>
+    <sheet name="config_gridConnections" sheetId="2" r:id="rId3"/>
     <sheet name="config_actors" sheetId="5" r:id="rId4"/>
     <sheet name="config_energyAssets" sheetId="4" r:id="rId5"/>
   </sheets>
@@ -774,7 +774,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -924,8 +924,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{493E8F37-4D53-4D4B-B589-A17DE4D133AF}">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q27" sqref="Q27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1440,7 +1440,7 @@
         <v>6</v>
       </c>
       <c r="H19" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I19" t="s">
         <v>89</v>

</xml_diff>

<commit_message>
Price band incentives from holon and gridOperator with TreeMap
*GridOperator is created from config excel and gridNodes linked to it, also from config excel,
*Alternative way of constructing and checking incentive price bands using TreeMap functionality,
*gridConnections receive (placeholder) price band incentive signals from gridOperator (communicated via gridNodes) and from their energyHolon if they have one,
*gridConnections check and combine the two signals with their supplier price by adding them up (for now).
</commit_message>
<xml_diff>
--- a/Base/db_backboneConfig.xlsx
+++ b/Base/db_backboneConfig.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\HOUJ\Documents\GitHub\HOLON\Base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{019B9943-555E-4C75-BD0B-5601DF22FF3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CF82D0E-F768-4982-9051-4C815F00CA97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{C61B0771-0652-4F35-8DF1-D2D550B8F66D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{C61B0771-0652-4F35-8DF1-D2D550B8F66D}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="111">
   <si>
     <t>id</t>
   </si>
@@ -360,6 +360,18 @@
   </si>
   <si>
     <t>gridNode</t>
+  </si>
+  <si>
+    <t>operator</t>
+  </si>
+  <si>
+    <t>o1</t>
+  </si>
+  <si>
+    <t>gridoperator</t>
+  </si>
+  <si>
+    <t>GRIDOPERATOR</t>
   </si>
 </sst>
 </file>
@@ -771,10 +783,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{243F788D-3AF5-439A-A91F-12D1BED9A308}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -783,7 +795,7 @@
     <col min="4" max="4" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -805,8 +817,11 @@
       <c r="G1" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -828,8 +843,11 @@
       <c r="G2" s="1">
         <v>1000</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -851,8 +869,11 @@
       <c r="G3" s="1">
         <v>1000</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -874,8 +895,11 @@
       <c r="G4" s="1">
         <v>1000</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -894,8 +918,11 @@
       <c r="G5" s="1">
         <v>500000</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1722,10 +1749,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F595F011-BCBA-42A0-B2C1-EC2B9C01AA0D}">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -2140,6 +2167,20 @@
       </c>
       <c r="E24" t="s">
         <v>93</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>109</v>
+      </c>
+      <c r="C25" t="s">
+        <v>110</v>
+      </c>
+      <c r="D25" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>